<commit_message>
include better fifo example
</commit_message>
<xml_diff>
--- a/blog-posts/improved-fifo-cogs-tracking.xlsx
+++ b/blog-posts/improved-fifo-cogs-tracking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rupum\Documents\GitHub\rupumped.github.io\blog-posts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick\Documents\GitHub\rupumped.github.io\blog-posts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2932B9CB-D01D-4FBA-83BD-DDF69D843FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6DF226-84EE-4C80-87A5-DD3FD4DB7F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{1551AAD6-5FC8-4B2F-8B2B-6343C0AFC811}"/>
+    <workbookView xWindow="-240" yWindow="-240" windowWidth="29280" windowHeight="15960" xr2:uid="{1551AAD6-5FC8-4B2F-8B2B-6343C0AFC811}"/>
   </bookViews>
   <sheets>
     <sheet name="Pie" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -836,32 +836,32 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.26171875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.26171875" customWidth="1"/>
-    <col min="13" max="13" width="17.83984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.26171875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.41796875" customWidth="1"/>
-    <col min="16" max="16" width="18.41796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.15625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.83984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -876,7 +876,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:20" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -935,7 +935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42077</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42077</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42077</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42078</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42079</v>
       </c>
@@ -1243,15 +1243,15 @@
         <v>4</v>
       </c>
       <c r="I7">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J7" s="3">
         <f>Sales[[#This Row],[COOGS]]+Sales[[#This Row],[CORGS]]</f>
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="K7">
         <f>SUMIF(H$3:H7,Sales[[#This Row],[Flavor]],I$3:I7)</f>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L7">
         <f>IFERROR(_xlfn.XMATCH(Sales[[#This Row],[Flavor]],H$2:H6,0,-1)-1,0)</f>
@@ -1275,11 +1275,11 @@
       </c>
       <c r="Q7">
         <f>MIN(Sales[[#This Row],[Qty of Oldest Order Left in Inventory Before This Sale]],Sales[[#This Row],[Qty Sold]])</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R7" s="3">
         <f>Sales[[#This Row],[Qty of Oldest Order Sold]]*Sales[[#This Row],[Cost Per Unit of Oldest Inventory]]</f>
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="S7">
         <f>Sales[[#This Row],[Qty Sold]]-Sales[[#This Row],[Qty of Oldest Order Sold]]</f>
@@ -1290,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42080</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>42081</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42082</v>
       </c>
@@ -1460,11 +1460,11 @@
       </c>
       <c r="J10" s="3">
         <f>Sales[[#This Row],[COOGS]]+Sales[[#This Row],[CORGS]]</f>
-        <v>1593</v>
+        <v>1589</v>
       </c>
       <c r="K10">
         <f>SUMIF(H$3:H10,Sales[[#This Row],[Flavor]],I$3:I10)</f>
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L10">
         <f>IFERROR(_xlfn.XMATCH(Sales[[#This Row],[Flavor]],H$2:H9,0,-1)-1,0)</f>
@@ -1472,7 +1472,7 @@
       </c>
       <c r="M10">
         <f>Sales[[#This Row],[Cumulative Sold]]-Sales[[#This Row],[Qty Sold]]</f>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N10" cm="1">
         <f t="array" ref="N10">_xlfn.XMATCH(Sales[[#This Row],[Total Qty Sold Before This Sale]],_xlfn._xlws.FILTER(Orders[Cumulative Ordered],(Orders[Flavor]=Sales[[#This Row],[Flavor]])*(Orders[Date]&lt;Sales[[#This Row],[Date]])),1,1)</f>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="O10" cm="1">
         <f t="array" ref="O10">INDEX(_xlfn._xlws.FILTER(Orders[Cumulative Ordered],(Orders[Flavor]=Sales[[#This Row],[Flavor]])*(Orders[Date]&lt;Sales[[#This Row],[Date]])),Sales[[#This Row],[Index of Oldest Order Still in Inventory Before This Sale]])-IF(Sales[[#This Row],[Index of Last Sale]]=0,0,INDEX(K$3:K9,Sales[[#This Row],[Index of Last Sale]]))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" s="3" cm="1">
         <f t="array" ref="P10">INDEX(_xlfn._xlws.FILTER(Orders[Cost Per Unit],Orders[Flavor]=Sales[[#This Row],[Flavor]]),Sales[[#This Row],[Index of Oldest Order Still in Inventory Before This Sale]])</f>
@@ -1488,22 +1488,22 @@
       </c>
       <c r="Q10">
         <f>MIN(Sales[[#This Row],[Qty of Oldest Order Left in Inventory Before This Sale]],Sales[[#This Row],[Qty Sold]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="3">
         <f>Sales[[#This Row],[Qty of Oldest Order Sold]]*Sales[[#This Row],[Cost Per Unit of Oldest Inventory]]</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="S10">
         <f>Sales[[#This Row],[Qty Sold]]-Sales[[#This Row],[Qty of Oldest Order Sold]]</f>
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T10" s="3" cm="1">
         <f t="array" ref="T10">_xlfn.LET(_xlpm.filteredSupply,_xlfn._xlws.FILTER(Orders[Qty Purchased],(Orders[Flavor]=Sales[[#This Row],[Flavor]])*(Orders[Date]&lt;Sales[[#This Row],[Date]])),_xlpm.filteredCostPerUnit,_xlfn._xlws.FILTER(Orders[Cost Per Unit],(Orders[Flavor]=Sales[[#This Row],[Flavor]])*(Orders[Date]&lt;Sales[[#This Row],[Date]])),IF(Sales[[#This Row],[Index of Oldest Order Still in Inventory Before This Sale]]&gt;=ROWS(_xlpm.filteredSupply),0,CORGS(Sales[[#This Row],[Additional Qty Needed]],Sales[[#This Row],[Index of Oldest Order Still in Inventory Before This Sale]]+1,_xlpm.filteredSupply,_xlpm.filteredCostPerUnit)))</f>
-        <v>1593</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42083</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42084</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42085</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42086</v>
       </c>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="K14">
         <f>SUMIF(H$3:H14,Sales[[#This Row],[Flavor]],I$3:I14)</f>
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L14">
         <f>IFERROR(_xlfn.XMATCH(Sales[[#This Row],[Flavor]],H$2:H13,0,-1)-1,0)</f>
@@ -1756,7 +1756,7 @@
       </c>
       <c r="M14">
         <f>Sales[[#This Row],[Cumulative Sold]]-Sales[[#This Row],[Qty Sold]]</f>
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N14" cm="1">
         <f t="array" ref="N14">_xlfn.XMATCH(Sales[[#This Row],[Total Qty Sold Before This Sale]],_xlfn._xlws.FILTER(Orders[Cumulative Ordered],(Orders[Flavor]=Sales[[#This Row],[Flavor]])*(Orders[Date]&lt;Sales[[#This Row],[Date]])),1,1)</f>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="O14" cm="1">
         <f t="array" ref="O14">INDEX(_xlfn._xlws.FILTER(Orders[Cumulative Ordered],(Orders[Flavor]=Sales[[#This Row],[Flavor]])*(Orders[Date]&lt;Sales[[#This Row],[Date]])),Sales[[#This Row],[Index of Oldest Order Still in Inventory Before This Sale]])-IF(Sales[[#This Row],[Index of Last Sale]]=0,0,INDEX(K$3:K13,Sales[[#This Row],[Index of Last Sale]]))</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P14" s="3" cm="1">
         <f t="array" ref="P14">INDEX(_xlfn._xlws.FILTER(Orders[Cost Per Unit],Orders[Flavor]=Sales[[#This Row],[Flavor]]),Sales[[#This Row],[Index of Oldest Order Still in Inventory Before This Sale]])</f>
@@ -1787,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42087</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42088</v>
       </c>
@@ -1898,29 +1898,29 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.578125" customWidth="1"/>
-    <col min="3" max="3" width="13.15625" customWidth="1"/>
-    <col min="4" max="4" width="12.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.15625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.68359375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.15625" customWidth="1"/>
-    <col min="10" max="10" width="14.15625" customWidth="1"/>
-    <col min="11" max="11" width="16.15625" customWidth="1"/>
-    <col min="12" max="12" width="27.26171875" customWidth="1"/>
-    <col min="13" max="13" width="30.578125" customWidth="1"/>
-    <col min="14" max="14" width="31.26171875" customWidth="1"/>
-    <col min="15" max="15" width="18.26171875" customWidth="1"/>
-    <col min="16" max="17" width="19.68359375" customWidth="1"/>
-    <col min="18" max="18" width="16.15625" customWidth="1"/>
-    <col min="19" max="19" width="19.68359375" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" customWidth="1"/>
+    <col min="13" max="13" width="30.5703125" customWidth="1"/>
+    <col min="14" max="14" width="31.28515625" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" customWidth="1"/>
+    <col min="16" max="17" width="19.7109375" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42077</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42077</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42077</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42109</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42110</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42111</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42142</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>1609.9999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>42143</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42144</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42176</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42177</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42178</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42209</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42210</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42211</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42237</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42238</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42239</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>4350</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42271</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>42272</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42273</v>
       </c>

</xml_diff>